<commit_message>
Solicitud de audios LE-08-01_REC230
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/ESCALETA_LE_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/ESCALETA_LE_08_02_CO.xlsx
@@ -986,22 +986,10 @@
     <t>Más información</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">La noticia </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">radial </t>
-    </r>
-  </si>
-  <si>
     <t>La noticia en vivo: vive una experiencia periodística</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La noticia </t>
   </si>
 </sst>
 </file>
@@ -1534,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,8 +1531,8 @@
     <col min="1" max="1" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.85546875" style="34" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" style="8" customWidth="1"/>
     <col min="7" max="7" width="81.7109375" style="8" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" style="6" customWidth="1"/>
@@ -3073,7 +3061,7 @@
       <c r="E26" s="13"/>
       <c r="F26" s="11"/>
       <c r="G26" s="20" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H26" s="14">
         <v>24</v>
@@ -3311,7 +3299,7 @@
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="41" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H30" s="14">
         <v>28</v>

</xml_diff>